<commit_message>
Auto-committed on 2022/04/22 週五
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L2-業務作業/FacClose.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L2-業務作業/FacClose.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\DB\GenTables\L2-業務作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6429C60-B35A-43C9-87DF-D5C903295AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F94BE75-9095-4CA0-8667-F661D011789F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="128">
   <si>
     <t>讀取Key條件</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -590,6 +590,10 @@
   </si>
   <si>
     <t xml:space="preserve">CustNo &gt;= ,AND CustNo &lt;= </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>findFacmNoMaxCloseNoFirst</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1932,11 +1936,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -2068,6 +2072,17 @@
         <v>114</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>